<commit_message>
init AFRM KPIs missing
</commit_message>
<xml_diff>
--- a/Business - Technology Services/SEZL.xlsx
+++ b/Business - Technology Services/SEZL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Business - Technology Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC4FE4-C851-4D39-ADBB-7242DEC22BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B122434-4033-4BCD-B339-0A5E6B6926D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="45" windowWidth="15480" windowHeight="15345" tabRatio="647" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="90" windowWidth="14010" windowHeight="15345" tabRatio="647" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,16 @@
     <sheet name="DoR" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Model!$L$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Model!$L$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Model!$L$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Model!$B$21</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Model!$B$22</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Model!$L$21:$P$21</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Model!$L$22:$P$22</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Model!$L$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Model!$L$21:$P$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Model!$L$22:$P$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Model!$L$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Model!$B$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Model!$B$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Model!$L$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Model!$L$3:$P$3</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Model!$L$4:$P$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1039,7 +1039,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="[$-407]mmm/\ yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1145,12 +1145,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1782,7 +1776,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1829,7 +1823,6 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1841,7 +1834,6 @@
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1963,6 +1955,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2020,8 +2014,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4767,6 +4768,9 @@
                 <c:pt idx="4">
                   <c:v>271.12788999999998</c:v>
                 </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>449.16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4900,7 +4904,7 @@
                   <c:v>0.70138919480622985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1</c:v>
+                  <c:v>0.65663517685325568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5990,7 +5994,7 @@
                   <c:v>77.581516999999963</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="#,##0">
-                  <c:v>118.27916999999999</c:v>
+                  <c:v>122.25797999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6114,7 +6118,7 @@
                   <c:v>9.3714636586471496</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52457923708813348</c:v>
+                  <c:v>0.57586477717366691</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8086,18 +8090,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.8</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8141,7 +8145,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>EPS exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8161,7 +8165,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>EPS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8192,18 +8196,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -8247,7 +8251,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Rev. Exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8267,7 +8271,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -15841,7 +15845,7 @@
       <c r="E2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="56" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="24"/>
@@ -15874,7 +15878,7 @@
       <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="121">
+      <c r="F3" s="119">
         <v>0.62009999999999998</v>
       </c>
       <c r="H3" t="s">
@@ -15905,7 +15909,7 @@
       <c r="E4" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="121">
+      <c r="F4" s="119">
         <v>0.14199999999999999</v>
       </c>
       <c r="H4" t="s">
@@ -16130,7 +16134,7 @@
       </c>
       <c r="C14" s="35">
         <f>C6/Model!H22</f>
-        <v>22.103975535168196</v>
+        <v>21.384615384615387</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="28"/>
@@ -16148,7 +16152,7 @@
       </c>
       <c r="C15" s="35">
         <f>C6/Model!I22</f>
-        <v>16.927400468384079</v>
+        <v>16.502283105022833</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -16157,7 +16161,7 @@
       </c>
       <c r="C16" s="5">
         <f>Model!H29</f>
-        <v>0.52457923708813348</v>
+        <v>0.57586477717366691</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -16166,7 +16170,7 @@
       </c>
       <c r="C17" s="5">
         <f>Model!I22/Model!H22-1</f>
-        <v>0.30581039755351669</v>
+        <v>0.29585798816568043</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>46</v>
@@ -16181,9 +16185,9 @@
       <c r="B18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <f>C14/(C16*100)</f>
-        <v>0.42136581039433235</v>
+        <v>0.37134786207225007</v>
       </c>
       <c r="L18" s="145"/>
       <c r="M18" s="146"/>
@@ -16193,9 +16197,9 @@
       <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <f>C15/(C17*100)</f>
-        <v>0.55352599531615965</v>
+        <v>0.55777716894977181</v>
       </c>
       <c r="L19" s="145"/>
       <c r="M19" s="146"/>
@@ -16207,7 +16211,7 @@
       </c>
       <c r="C20" s="5">
         <f>Model!H4/Model!G4-1</f>
-        <v>0.99578785271072046</v>
+        <v>1.0343312650029444</v>
       </c>
       <c r="L20" s="145"/>
       <c r="M20" s="146"/>
@@ -16219,7 +16223,7 @@
       </c>
       <c r="C21" s="5">
         <f>Model!I4/Model!H4-1</f>
-        <v>0.27293770566209008</v>
+        <v>0.2601522842639592</v>
       </c>
       <c r="L21" s="145"/>
       <c r="M21" s="146"/>
@@ -16289,7 +16293,7 @@
       <c r="B27" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="116" t="s">
         <v>197</v>
       </c>
       <c r="E27" t="s">
@@ -16393,26 +16397,26 @@
       <c r="C36" s="22"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="55"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="55"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="55"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16428,10 +16432,10 @@
   <dimension ref="A1:Z83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16517,57 +16521,64 @@
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="124">
+      <c r="C3" s="122">
         <f>49.659042+9.129231</f>
         <v>58.788273000000004</v>
       </c>
-      <c r="D3" s="124">
+      <c r="D3" s="122">
         <f>98.200184+16.616451</f>
         <v>114.81663499999999</v>
       </c>
-      <c r="E3" s="124">
+      <c r="E3" s="122">
         <v>125.570441</v>
       </c>
-      <c r="F3" s="124">
+      <c r="F3" s="122">
         <v>159.35677200000001</v>
       </c>
-      <c r="G3" s="125">
+      <c r="G3" s="123">
         <v>271.12788999999998</v>
       </c>
-      <c r="H3" s="42"/>
+      <c r="H3" s="164">
+        <f>H4</f>
+        <v>449.16</v>
+      </c>
+      <c r="I3" s="166">
+        <f>I4</f>
+        <v>566.01</v>
+      </c>
       <c r="L3" s="17">
         <v>34.673431000000001</v>
       </c>
-      <c r="M3" s="124">
+      <c r="M3" s="122">
         <v>34.937665000000003</v>
       </c>
-      <c r="N3" s="124">
+      <c r="N3" s="122">
         <v>40.844200999999998</v>
       </c>
-      <c r="O3" s="124">
+      <c r="O3" s="122">
         <f>F3-N3-M3-L3</f>
         <v>48.901474999999998</v>
       </c>
-      <c r="P3" s="124">
+      <c r="P3" s="122">
         <v>46.978634</v>
       </c>
-      <c r="Q3" s="124">
+      <c r="Q3" s="122">
         <v>55.968505</v>
       </c>
-      <c r="R3" s="124">
+      <c r="R3" s="122">
         <v>69.957690999999997</v>
       </c>
-      <c r="S3" s="124">
+      <c r="S3" s="122">
         <f>G3-R3-Q3-P3</f>
         <v>98.223059999999975</v>
       </c>
-      <c r="T3" s="124">
+      <c r="T3" s="122">
         <v>104.91200000000001</v>
       </c>
-      <c r="U3" s="124">
+      <c r="U3" s="122">
         <v>98.701999999999998</v>
       </c>
-      <c r="V3" s="125">
+      <c r="V3" s="123">
         <v>116.79600000000001</v>
       </c>
     </row>
@@ -16575,95 +16586,98 @@
       <c r="B4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="125">
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="123">
         <v>220.79</v>
       </c>
       <c r="H4" s="41">
-        <v>440.65</v>
-      </c>
-      <c r="I4">
-        <v>560.91999999999996</v>
+        <v>449.16</v>
+      </c>
+      <c r="I4" s="125">
+        <v>566.01</v>
       </c>
       <c r="L4" s="17"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124">
+      <c r="M4" s="122"/>
+      <c r="N4" s="122"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122"/>
+      <c r="Q4" s="122"/>
+      <c r="R4" s="122">
         <v>52.63</v>
       </c>
-      <c r="S4" s="124">
+      <c r="S4" s="122">
         <v>65.180000000000007</v>
       </c>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124">
+      <c r="T4" s="122"/>
+      <c r="U4" s="122">
         <v>93.33</v>
       </c>
-      <c r="V4" s="125">
+      <c r="V4" s="123">
         <v>104.7</v>
       </c>
-      <c r="W4" s="124">
-        <v>132.35</v>
+      <c r="W4" s="122">
+        <v>128.91</v>
+      </c>
+      <c r="X4" s="169">
+        <v>128.1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="124">
+      <c r="C5" s="122">
         <v>30.689461999999999</v>
       </c>
-      <c r="D5" s="124">
+      <c r="D5" s="122">
         <v>56.831367999999998</v>
       </c>
-      <c r="E5" s="124">
+      <c r="E5" s="122">
         <v>51.217083000000002</v>
       </c>
-      <c r="F5" s="124">
+      <c r="F5" s="122">
         <v>46.373914999999997</v>
       </c>
-      <c r="G5" s="125">
+      <c r="G5" s="123">
         <v>51.764963999999999</v>
       </c>
-      <c r="H5" s="41"/>
+      <c r="H5" s="165"/>
       <c r="L5" s="17">
         <v>11.57399</v>
       </c>
-      <c r="M5" s="124">
+      <c r="M5" s="122">
         <v>12.017071</v>
       </c>
-      <c r="N5" s="124">
+      <c r="N5" s="122">
         <v>11.079174</v>
       </c>
-      <c r="O5" s="124">
+      <c r="O5" s="122">
         <f t="shared" ref="O5:O10" si="0">F5-N5-M5-L5</f>
         <v>11.703679999999993</v>
       </c>
-      <c r="P5" s="124">
+      <c r="P5" s="122">
         <v>11.025040000000001</v>
       </c>
-      <c r="Q5" s="124">
+      <c r="Q5" s="122">
         <v>12.736523</v>
       </c>
-      <c r="R5" s="124">
+      <c r="R5" s="122">
         <v>13.423723000000001</v>
       </c>
-      <c r="S5" s="124">
+      <c r="S5" s="122">
         <f t="shared" ref="S5:S10" si="1">G5-R5-Q5-P5</f>
         <v>14.579677999999998</v>
       </c>
-      <c r="T5" s="124">
+      <c r="T5" s="122">
         <v>15.048</v>
       </c>
-      <c r="U5" s="124">
+      <c r="U5" s="122">
         <v>11.680999999999999</v>
       </c>
-      <c r="V5" s="125">
+      <c r="V5" s="123">
         <v>14.32</v>
       </c>
     </row>
@@ -16671,55 +16685,55 @@
       <c r="B6" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="124">
+      <c r="C6" s="122">
         <v>22.489626000000001</v>
       </c>
-      <c r="D6" s="124">
+      <c r="D6" s="122">
         <v>43.476143</v>
       </c>
-      <c r="E6" s="124">
+      <c r="E6" s="122">
         <v>40.776825000000002</v>
       </c>
-      <c r="F6" s="124">
+      <c r="F6" s="122">
         <v>39.207768000000002</v>
       </c>
-      <c r="G6" s="125">
+      <c r="G6" s="123">
         <v>51.364347000000002</v>
       </c>
-      <c r="H6" s="41"/>
+      <c r="H6" s="165"/>
       <c r="L6" s="17">
         <v>8.2385859999999997</v>
       </c>
-      <c r="M6" s="124">
+      <c r="M6" s="122">
         <v>7.9459479999999996</v>
       </c>
-      <c r="N6" s="124">
+      <c r="N6" s="122">
         <v>9.9368040000000004</v>
       </c>
-      <c r="O6" s="124">
+      <c r="O6" s="122">
         <f t="shared" si="0"/>
         <v>13.086429999999998</v>
       </c>
-      <c r="P6" s="124">
+      <c r="P6" s="122">
         <v>11.787146</v>
       </c>
-      <c r="Q6" s="124">
+      <c r="Q6" s="122">
         <v>10.741618000000001</v>
       </c>
-      <c r="R6" s="124">
+      <c r="R6" s="122">
         <v>12.761438</v>
       </c>
-      <c r="S6" s="124">
+      <c r="S6" s="122">
         <f t="shared" si="1"/>
         <v>16.074145000000001</v>
       </c>
-      <c r="T6" s="124">
+      <c r="T6" s="122">
         <v>15.317</v>
       </c>
-      <c r="U6" s="124">
+      <c r="U6" s="122">
         <v>14.243</v>
       </c>
-      <c r="V6" s="125">
+      <c r="V6" s="123">
         <v>17.434999999999999</v>
       </c>
     </row>
@@ -16727,55 +16741,55 @@
       <c r="B7" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="124">
+      <c r="C7" s="122">
         <v>2.454113</v>
       </c>
-      <c r="D7" s="124">
+      <c r="D7" s="122">
         <v>5.5498440000000002</v>
       </c>
-      <c r="E7" s="124">
+      <c r="E7" s="122">
         <v>8.1900220000000008</v>
       </c>
-      <c r="F7" s="124">
+      <c r="F7" s="122">
         <v>7.8159150000000004</v>
       </c>
-      <c r="G7" s="125">
+      <c r="G7" s="123">
         <v>9.5951059999999995</v>
       </c>
-      <c r="H7" s="41"/>
+      <c r="H7" s="165"/>
       <c r="L7" s="17">
         <v>1.7491760000000001</v>
       </c>
-      <c r="M7" s="124">
+      <c r="M7" s="122">
         <v>1.9036299999999999</v>
       </c>
-      <c r="N7" s="124">
+      <c r="N7" s="122">
         <v>2.0025149999999998</v>
       </c>
-      <c r="O7" s="124">
+      <c r="O7" s="122">
         <f t="shared" si="0"/>
         <v>2.1605940000000006</v>
       </c>
-      <c r="P7" s="124">
+      <c r="P7" s="122">
         <v>2.1571720000000001</v>
       </c>
-      <c r="Q7" s="124">
+      <c r="Q7" s="122">
         <v>2.1802329999999999</v>
       </c>
-      <c r="R7" s="124">
+      <c r="R7" s="122">
         <v>2.3864899999999998</v>
       </c>
-      <c r="S7" s="124">
+      <c r="S7" s="122">
         <f t="shared" si="1"/>
         <v>2.8712109999999997</v>
       </c>
-      <c r="T7" s="124">
+      <c r="T7" s="122">
         <v>3.3740000000000001</v>
       </c>
-      <c r="U7" s="124">
+      <c r="U7" s="122">
         <v>3.4279999999999999</v>
       </c>
-      <c r="V7" s="125">
+      <c r="V7" s="123">
         <v>3.7050000000000001</v>
       </c>
     </row>
@@ -16783,55 +16797,55 @@
       <c r="B8" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="124">
+      <c r="C8" s="122">
         <v>4.2749290000000002</v>
       </c>
-      <c r="D8" s="124">
+      <c r="D8" s="122">
         <v>9.2518539999999998</v>
       </c>
-      <c r="E8" s="124">
+      <c r="E8" s="122">
         <v>18.972024999999999</v>
       </c>
-      <c r="F8" s="124">
+      <c r="F8" s="122">
         <v>11.984019</v>
       </c>
-      <c r="G8" s="125">
+      <c r="G8" s="123">
         <v>9.7397629999999999</v>
       </c>
       <c r="H8" s="39"/>
       <c r="L8" s="17">
         <v>3.1991740000000002</v>
       </c>
-      <c r="M8" s="124">
+      <c r="M8" s="122">
         <v>3.3136619999999999</v>
       </c>
-      <c r="N8" s="124">
+      <c r="N8" s="122">
         <v>3.6153390000000001</v>
       </c>
-      <c r="O8" s="124">
+      <c r="O8" s="122">
         <f t="shared" si="0"/>
         <v>1.8558439999999994</v>
       </c>
-      <c r="P8" s="124">
+      <c r="P8" s="122">
         <v>0.65487499999999998</v>
       </c>
-      <c r="Q8" s="124">
+      <c r="Q8" s="122">
         <v>0.995089</v>
       </c>
-      <c r="R8" s="124">
+      <c r="R8" s="122">
         <v>2.7256149999999999</v>
       </c>
-      <c r="S8" s="124">
+      <c r="S8" s="122">
         <f t="shared" si="1"/>
         <v>5.3641840000000007</v>
       </c>
-      <c r="T8" s="124">
+      <c r="T8" s="122">
         <v>5.3460000000000001</v>
       </c>
-      <c r="U8" s="124">
+      <c r="U8" s="122">
         <v>8.7720000000000002</v>
       </c>
-      <c r="V8" s="125">
+      <c r="V8" s="123">
         <v>8.7750000000000004</v>
       </c>
     </row>
@@ -16839,55 +16853,55 @@
       <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="124">
+      <c r="C9" s="122">
         <v>7.2145349999999997</v>
       </c>
-      <c r="D9" s="124">
+      <c r="D9" s="122">
         <v>15.768583</v>
       </c>
-      <c r="E9" s="124">
+      <c r="E9" s="122">
         <v>16.411912000000001</v>
       </c>
-      <c r="F9" s="124">
+      <c r="F9" s="122">
         <v>8.5877809999999997</v>
       </c>
-      <c r="G9" s="125">
+      <c r="G9" s="123">
         <v>11.403468</v>
       </c>
       <c r="H9" s="39"/>
       <c r="L9" s="17">
         <v>2.7982100000000001</v>
       </c>
-      <c r="M9" s="124">
+      <c r="M9" s="122">
         <v>1.6976290000000001</v>
       </c>
-      <c r="N9" s="124">
+      <c r="N9" s="122">
         <v>2.1840760000000001</v>
       </c>
-      <c r="O9" s="124">
+      <c r="O9" s="122">
         <f t="shared" si="0"/>
         <v>1.9078659999999994</v>
       </c>
-      <c r="P9" s="124">
+      <c r="P9" s="122">
         <v>2.3797779999999999</v>
       </c>
-      <c r="Q9" s="124">
+      <c r="Q9" s="122">
         <v>2.521782</v>
       </c>
-      <c r="R9" s="124">
+      <c r="R9" s="122">
         <v>2.4169510000000001</v>
       </c>
-      <c r="S9" s="124">
+      <c r="S9" s="122">
         <f t="shared" si="1"/>
         <v>4.0849569999999993</v>
       </c>
-      <c r="T9" s="124">
+      <c r="T9" s="122">
         <v>3.1309999999999998</v>
       </c>
-      <c r="U9" s="124">
+      <c r="U9" s="122">
         <v>3.8460000000000001</v>
       </c>
-      <c r="V9" s="125">
+      <c r="V9" s="123">
         <v>4.8230000000000004</v>
       </c>
     </row>
@@ -16895,55 +16909,55 @@
       <c r="B10" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="124">
+      <c r="C10" s="122">
         <v>19.587917999999998</v>
       </c>
-      <c r="D10" s="124">
+      <c r="D10" s="122">
         <v>52.621682</v>
       </c>
-      <c r="E10" s="124">
+      <c r="E10" s="122">
         <v>29.437179</v>
       </c>
-      <c r="F10" s="124">
+      <c r="F10" s="122">
         <v>23.186972999999998</v>
       </c>
-      <c r="G10" s="125">
+      <c r="G10" s="123">
         <v>55.014676000000001</v>
       </c>
       <c r="H10" s="9"/>
       <c r="L10" s="17">
         <v>1.694364</v>
       </c>
-      <c r="M10" s="124">
+      <c r="M10" s="122">
         <v>4.2964339999999996</v>
       </c>
-      <c r="N10" s="124">
+      <c r="N10" s="122">
         <v>6.6765480000000004</v>
       </c>
-      <c r="O10" s="124">
+      <c r="O10" s="122">
         <f t="shared" si="0"/>
         <v>10.519626999999998</v>
       </c>
-      <c r="P10" s="124">
+      <c r="P10" s="122">
         <v>5.1399660000000003</v>
       </c>
-      <c r="Q10" s="124">
+      <c r="Q10" s="122">
         <v>10.09388</v>
       </c>
-      <c r="R10" s="124">
+      <c r="R10" s="122">
         <v>15.402303</v>
       </c>
-      <c r="S10" s="124">
+      <c r="S10" s="122">
         <f t="shared" si="1"/>
         <v>24.378527000000005</v>
       </c>
-      <c r="T10" s="124">
+      <c r="T10" s="122">
         <v>12.801</v>
       </c>
-      <c r="U10" s="124">
+      <c r="U10" s="122">
         <v>20.646000000000001</v>
       </c>
-      <c r="V10" s="125">
+      <c r="V10" s="123">
         <v>32.177</v>
       </c>
     </row>
@@ -16951,110 +16965,113 @@
       <c r="B11" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="124"/>
-      <c r="D11" s="124"/>
-      <c r="E11" s="124">
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122">
         <v>-11</v>
       </c>
-      <c r="F11" s="124"/>
-      <c r="G11" s="125"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="39"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-      <c r="Q11" s="124"/>
-      <c r="R11" s="124"/>
-      <c r="S11" s="124"/>
-      <c r="T11" s="124"/>
-      <c r="U11" s="124"/>
-      <c r="V11" s="125"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="122"/>
+      <c r="O11" s="122"/>
+      <c r="P11" s="122"/>
+      <c r="Q11" s="122"/>
+      <c r="R11" s="122"/>
+      <c r="S11" s="122"/>
+      <c r="T11" s="122"/>
+      <c r="U11" s="122"/>
+      <c r="V11" s="123"/>
     </row>
     <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="122">
+      <c r="C12" s="120">
         <f t="shared" ref="C12:E12" si="2">C3-SUM(C5:C11)</f>
         <v>-27.922309999999996</v>
       </c>
-      <c r="D12" s="122">
+      <c r="D12" s="120">
         <f t="shared" si="2"/>
         <v>-68.682839000000001</v>
       </c>
-      <c r="E12" s="122">
+      <c r="E12" s="120">
         <f t="shared" si="2"/>
         <v>-28.434604999999991</v>
       </c>
-      <c r="F12" s="122">
+      <c r="F12" s="120">
         <f>F3-SUM(F5:F11)</f>
         <v>22.200400999999999</v>
       </c>
-      <c r="G12" s="126">
+      <c r="G12" s="124">
         <f>G3-SUM(G5:G11)</f>
         <v>82.245565999999968</v>
       </c>
       <c r="H12" s="10">
         <f>H3-SUM(H8:H11)</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="10"/>
+        <v>449.16</v>
+      </c>
+      <c r="I12" s="10">
+        <f>I3-SUM(I8:I11)</f>
+        <v>566.01</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="2">
         <f t="shared" ref="L12" si="3">L3-SUM(L5:L11)</f>
         <v>5.4199310000000018</v>
       </c>
-      <c r="M12" s="122">
+      <c r="M12" s="120">
         <f>M3-SUM(M5:M11)</f>
         <v>3.7632910000000024</v>
       </c>
-      <c r="N12" s="122">
+      <c r="N12" s="120">
         <f t="shared" ref="N12" si="4">N3-SUM(N5:N11)</f>
         <v>5.3497449999999986</v>
       </c>
-      <c r="O12" s="122">
+      <c r="O12" s="120">
         <f t="shared" ref="O12" si="5">O3-SUM(O5:O11)</f>
         <v>7.6674340000000072</v>
       </c>
-      <c r="P12" s="122">
+      <c r="P12" s="120">
         <f t="shared" ref="P12" si="6">P3-SUM(P5:P11)</f>
         <v>13.834657</v>
       </c>
-      <c r="Q12" s="122">
+      <c r="Q12" s="120">
         <f t="shared" ref="Q12" si="7">Q3-SUM(Q5:Q11)</f>
         <v>16.699379999999998</v>
       </c>
-      <c r="R12" s="122">
+      <c r="R12" s="120">
         <f>R3-SUM(R5:R11)</f>
         <v>20.841171000000003</v>
       </c>
-      <c r="S12" s="122">
+      <c r="S12" s="120">
         <f>S3-SUM(S5:S11)</f>
         <v>30.870357999999968</v>
       </c>
-      <c r="T12" s="122">
+      <c r="T12" s="120">
         <f>T3-SUM(T5:T11)</f>
         <v>49.894999999999996</v>
       </c>
-      <c r="U12" s="122">
+      <c r="U12" s="120">
         <f t="shared" ref="U12:Y12" si="8">U3-SUM(U5:U11)</f>
         <v>36.085999999999999</v>
       </c>
-      <c r="V12" s="126">
+      <c r="V12" s="124">
         <f t="shared" si="8"/>
         <v>35.561000000000007</v>
       </c>
-      <c r="W12" s="122">
+      <c r="W12" s="120">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="X12" s="122">
+      <c r="X12" s="120">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y12" s="122">
+      <c r="Y12" s="120">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -17063,55 +17080,55 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="124">
+      <c r="C13" s="122">
         <v>-4.3031750000000004</v>
       </c>
-      <c r="D13" s="124">
+      <c r="D13" s="122">
         <v>-5.2692839999999999</v>
       </c>
-      <c r="E13" s="124">
+      <c r="E13" s="122">
         <v>-8.6007160000000002</v>
       </c>
-      <c r="F13" s="124">
+      <c r="F13" s="122">
         <v>-15.96838</v>
       </c>
-      <c r="G13" s="125">
+      <c r="G13" s="123">
         <v>-13.761645</v>
       </c>
       <c r="H13" s="39"/>
       <c r="L13" s="17">
         <v>-3.3770470000000001</v>
       </c>
-      <c r="M13" s="124">
+      <c r="M13" s="122">
         <v>-3.933446</v>
       </c>
-      <c r="N13" s="124">
+      <c r="N13" s="122">
         <v>-4.1432580000000003</v>
       </c>
-      <c r="O13" s="124">
+      <c r="O13" s="122">
         <f>F13-N13-M13-L13</f>
         <v>-4.5146290000000002</v>
       </c>
-      <c r="P13" s="124">
+      <c r="P13" s="122">
         <v>-4.081442</v>
       </c>
-      <c r="Q13" s="124">
+      <c r="Q13" s="122">
         <v>-2.911133</v>
       </c>
-      <c r="R13" s="124">
+      <c r="R13" s="122">
         <v>-3.327998</v>
       </c>
-      <c r="S13" s="124">
+      <c r="S13" s="122">
         <f t="shared" ref="S13:S15" si="9">G13-R13-Q13-P13</f>
         <v>-3.441072000000001</v>
       </c>
-      <c r="T13" s="124">
+      <c r="T13" s="122">
         <v>-2.9140000000000001</v>
       </c>
-      <c r="U13" s="124">
+      <c r="U13" s="122">
         <v>-3.5009999999999999</v>
       </c>
-      <c r="V13" s="125">
+      <c r="V13" s="123">
         <v>-3.923</v>
       </c>
     </row>
@@ -17119,55 +17136,55 @@
       <c r="B14" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="124">
+      <c r="C14" s="122">
         <v>-0.12629099999999999</v>
       </c>
-      <c r="D14" s="124">
+      <c r="D14" s="122">
         <v>-6.5144999999999995E-2</v>
       </c>
-      <c r="E14" s="124">
+      <c r="E14" s="122">
         <v>-0.225606</v>
       </c>
-      <c r="F14" s="124">
+      <c r="F14" s="122">
         <v>1.9334499999999999</v>
       </c>
-      <c r="G14" s="125">
+      <c r="G14" s="123">
         <v>0.354487</v>
       </c>
       <c r="H14" s="39"/>
       <c r="L14" s="17">
         <v>0.113487</v>
       </c>
-      <c r="M14" s="124">
+      <c r="M14" s="122">
         <v>1.0787530000000001</v>
       </c>
-      <c r="N14" s="124">
+      <c r="N14" s="122">
         <v>1.456E-2</v>
       </c>
-      <c r="O14" s="124">
+      <c r="O14" s="122">
         <f>F14-N14-M14-L14</f>
         <v>0.72664999999999991</v>
       </c>
-      <c r="P14" s="124">
+      <c r="P14" s="122">
         <v>-9.1560000000000002E-2</v>
       </c>
-      <c r="Q14" s="124">
+      <c r="Q14" s="122">
         <v>5.0126999999999998E-2</v>
       </c>
-      <c r="R14" s="124">
+      <c r="R14" s="122">
         <v>9.6057000000000003E-2</v>
       </c>
-      <c r="S14" s="124">
+      <c r="S14" s="122">
         <f t="shared" si="9"/>
         <v>0.29986299999999999</v>
       </c>
-      <c r="T14" s="124">
+      <c r="T14" s="122">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="U14" s="124">
+      <c r="U14" s="122">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="V14" s="125">
+      <c r="V14" s="123">
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
@@ -17175,20 +17192,20 @@
       <c r="B15" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="124">
+      <c r="C15" s="122">
         <v>0</v>
       </c>
-      <c r="D15" s="124">
+      <c r="D15" s="122">
         <v>-1.092679</v>
       </c>
-      <c r="E15" s="124">
+      <c r="E15" s="122">
         <f>-0.813806+0.050424</f>
         <v>-0.76338200000000001</v>
       </c>
-      <c r="F15" s="124">
+      <c r="F15" s="122">
         <v>-0.45596199999999998</v>
       </c>
-      <c r="G15" s="125">
+      <c r="G15" s="123">
         <f>-1.261556-0.259706</f>
         <v>-1.5212619999999999</v>
       </c>
@@ -17196,114 +17213,118 @@
       <c r="L15" s="17">
         <v>-0.42020099999999999</v>
       </c>
-      <c r="M15" s="124">
+      <c r="M15" s="122">
         <v>0.25170599999999999</v>
       </c>
-      <c r="N15" s="124">
+      <c r="N15" s="122">
         <v>8.9227000000000001E-2</v>
       </c>
-      <c r="O15" s="124">
+      <c r="O15" s="122">
         <f>F15-N15-M15-L15</f>
         <v>-0.37669399999999992</v>
       </c>
-      <c r="P15" s="124">
+      <c r="P15" s="122">
         <v>-1.2615559999999999</v>
       </c>
-      <c r="Q15" s="124">
+      <c r="Q15" s="122">
         <v>-0.25970599999999999</v>
       </c>
-      <c r="R15" s="124">
+      <c r="R15" s="122">
         <v>0</v>
       </c>
-      <c r="S15" s="124">
+      <c r="S15" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="T15" s="124"/>
-      <c r="U15" s="124"/>
-      <c r="V15" s="125"/>
+      <c r="T15" s="122"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="123"/>
     </row>
     <row r="16" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="122">
+      <c r="C16" s="120">
         <f>C12+SUM(C13:C15)</f>
         <v>-32.351775999999994</v>
       </c>
-      <c r="D16" s="122">
-        <f t="shared" ref="D16:H16" si="10">D12+SUM(D13:D15)</f>
+      <c r="D16" s="120">
+        <f t="shared" ref="D16:I16" si="10">D12+SUM(D13:D15)</f>
         <v>-75.109947000000005</v>
       </c>
-      <c r="E16" s="122">
+      <c r="E16" s="120">
         <f t="shared" si="10"/>
         <v>-38.024308999999988</v>
       </c>
-      <c r="F16" s="122">
+      <c r="F16" s="120">
         <f t="shared" si="10"/>
         <v>7.7095090000000006</v>
       </c>
-      <c r="G16" s="126">
+      <c r="G16" s="124">
         <f t="shared" si="10"/>
         <v>67.317145999999966</v>
       </c>
       <c r="H16" s="10">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>449.16</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="10"/>
+        <v>566.01</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ref="L16" si="11">L12+SUM(L13:L15)</f>
         <v>1.7361700000000018</v>
       </c>
-      <c r="M16" s="122">
+      <c r="M16" s="120">
         <f>M12+SUM(M13:M15)</f>
         <v>1.1603040000000022</v>
       </c>
-      <c r="N16" s="122">
+      <c r="N16" s="120">
         <f t="shared" ref="N16" si="12">N12+SUM(N13:N15)</f>
         <v>1.3102739999999988</v>
       </c>
-      <c r="O16" s="122">
+      <c r="O16" s="120">
         <f t="shared" ref="O16" si="13">O12+SUM(O13:O15)</f>
         <v>3.5027610000000067</v>
       </c>
-      <c r="P16" s="122">
+      <c r="P16" s="120">
         <f t="shared" ref="P16" si="14">P12+SUM(P13:P15)</f>
         <v>8.4000990000000009</v>
       </c>
-      <c r="Q16" s="122">
+      <c r="Q16" s="120">
         <f t="shared" ref="Q16:R16" si="15">Q12+SUM(Q13:Q15)</f>
         <v>13.578667999999997</v>
       </c>
-      <c r="R16" s="122">
+      <c r="R16" s="120">
         <f t="shared" si="15"/>
         <v>17.609230000000004</v>
       </c>
-      <c r="S16" s="122">
+      <c r="S16" s="120">
         <f t="shared" ref="S16:Y16" si="16">S12+SUM(S13:S15)</f>
         <v>27.729148999999968</v>
       </c>
-      <c r="T16" s="122">
+      <c r="T16" s="120">
         <f t="shared" si="16"/>
         <v>47.005999999999993</v>
       </c>
-      <c r="U16" s="122">
+      <c r="U16" s="120">
         <f>U12+SUM(U13:U15)</f>
         <v>32.671999999999997</v>
       </c>
-      <c r="V16" s="126">
+      <c r="V16" s="124">
         <f t="shared" si="16"/>
         <v>31.632000000000009</v>
       </c>
-      <c r="W16" s="126">
+      <c r="W16" s="161">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="X16" s="126">
+      <c r="X16" s="161">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="Y16" s="126">
+      <c r="Y16" s="161">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
@@ -17312,55 +17333,55 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="124">
+      <c r="C17" s="122">
         <v>3.0963999999999998E-2</v>
       </c>
-      <c r="D17" s="124">
+      <c r="D17" s="122">
         <v>5.8416000000000003E-2</v>
       </c>
-      <c r="E17" s="124">
+      <c r="E17" s="122">
         <v>6.9446999999999995E-2</v>
       </c>
-      <c r="F17" s="124">
+      <c r="F17" s="122">
         <v>0.611487</v>
       </c>
-      <c r="G17" s="125">
+      <c r="G17" s="123">
         <v>-11.205164999999999</v>
       </c>
       <c r="H17" s="39"/>
       <c r="L17" s="17">
         <v>1.1624000000000001E-2</v>
       </c>
-      <c r="M17" s="124">
+      <c r="M17" s="122">
         <v>2.0525999999999999E-2</v>
       </c>
-      <c r="N17" s="124">
+      <c r="N17" s="122">
         <v>1.5873999999999999E-2</v>
       </c>
-      <c r="O17" s="124">
+      <c r="O17" s="122">
         <f>F17-N17-M17-L17</f>
         <v>0.56346299999999994</v>
       </c>
-      <c r="P17" s="124">
+      <c r="P17" s="122">
         <v>0.393094</v>
       </c>
-      <c r="Q17" s="124">
+      <c r="Q17" s="122">
         <v>-16.123213</v>
       </c>
-      <c r="R17" s="124">
+      <c r="R17" s="122">
         <v>2.1629890000000001</v>
       </c>
-      <c r="S17" s="124">
+      <c r="S17" s="122">
         <f t="shared" ref="S17:S18" si="17">G17-R17-Q17-P17</f>
         <v>2.361965000000001</v>
       </c>
-      <c r="T17" s="124">
+      <c r="T17" s="122">
         <v>10.842000000000001</v>
       </c>
-      <c r="U17" s="124">
+      <c r="U17" s="122">
         <v>5.0679999999999996</v>
       </c>
-      <c r="V17" s="125">
+      <c r="V17" s="123">
         <v>4.9610000000000003</v>
       </c>
     </row>
@@ -17368,55 +17389,55 @@
       <c r="B18" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="124">
+      <c r="C18" s="122">
         <v>0.49450499999999997</v>
       </c>
-      <c r="D18" s="124">
+      <c r="D18" s="122">
         <v>6.9405999999999995E-2</v>
       </c>
-      <c r="E18" s="124">
+      <c r="E18" s="122">
         <v>-1.2078850000000001</v>
       </c>
-      <c r="F18" s="124">
+      <c r="F18" s="122">
         <v>-3.0249999999999999E-3</v>
       </c>
-      <c r="G18" s="125">
+      <c r="G18" s="123">
         <v>0.94079400000000002</v>
       </c>
       <c r="H18" s="39"/>
       <c r="L18" s="17">
         <v>0.14580799999999999</v>
       </c>
-      <c r="M18" s="124">
+      <c r="M18" s="122">
         <v>-0.30468699999999999</v>
       </c>
-      <c r="N18" s="124">
+      <c r="N18" s="122">
         <v>0.35846499999999998</v>
       </c>
-      <c r="O18" s="124">
+      <c r="O18" s="122">
         <f>F18-N18-M18-L18</f>
         <v>-0.20261099999999999</v>
       </c>
-      <c r="P18" s="124">
+      <c r="P18" s="122">
         <v>-1.451E-3</v>
       </c>
-      <c r="Q18" s="124">
+      <c r="Q18" s="122">
         <v>-7.5401999999999997E-2</v>
       </c>
-      <c r="R18" s="124">
+      <c r="R18" s="122">
         <v>-7.1597999999999995E-2</v>
       </c>
-      <c r="S18" s="124">
+      <c r="S18" s="122">
         <f t="shared" si="17"/>
         <v>1.089245</v>
       </c>
-      <c r="T18" s="124">
+      <c r="T18" s="122">
         <v>-9.2999999999999999E-2</v>
       </c>
-      <c r="U18" s="124">
+      <c r="U18" s="122">
         <v>0.72899999999999998</v>
       </c>
-      <c r="V18" s="125">
+      <c r="V18" s="123">
         <v>0.33900000000000002</v>
       </c>
     </row>
@@ -17424,83 +17445,87 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="122">
+      <c r="C19" s="120">
         <f t="shared" ref="C19:F19" si="18">C16-SUM(C17:C18)</f>
         <v>-32.877244999999995</v>
       </c>
-      <c r="D19" s="122">
+      <c r="D19" s="120">
         <f t="shared" si="18"/>
         <v>-75.237769</v>
       </c>
-      <c r="E19" s="122">
+      <c r="E19" s="120">
         <f t="shared" si="18"/>
         <v>-36.885870999999987</v>
       </c>
-      <c r="F19" s="122">
+      <c r="F19" s="120">
         <f t="shared" si="18"/>
         <v>7.1010470000000003</v>
       </c>
-      <c r="G19" s="126">
+      <c r="G19" s="124">
         <f>G16-SUM(G17:G18)</f>
         <v>77.581516999999963</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="51">
         <f>H22*H20</f>
-        <v>118.27916999999999</v>
+        <v>122.25797999999999</v>
+      </c>
+      <c r="I19" s="51">
+        <f>I22*I20</f>
+        <v>0</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" ref="L19:M19" si="19">L16-SUM(L17:L18)</f>
         <v>1.5787380000000018</v>
       </c>
-      <c r="M19" s="122">
+      <c r="M19" s="120">
         <f t="shared" si="19"/>
         <v>1.4444650000000023</v>
       </c>
-      <c r="N19" s="122">
+      <c r="N19" s="120">
         <f t="shared" ref="N19" si="20">N16-SUM(N17:N18)</f>
         <v>0.93593499999999885</v>
       </c>
-      <c r="O19" s="122">
+      <c r="O19" s="120">
         <f t="shared" ref="O19" si="21">O16-SUM(O17:O18)</f>
         <v>3.1419090000000067</v>
       </c>
-      <c r="P19" s="122">
+      <c r="P19" s="120">
         <f t="shared" ref="P19" si="22">P16-SUM(P17:P18)</f>
         <v>8.0084560000000007</v>
       </c>
-      <c r="Q19" s="122">
+      <c r="Q19" s="120">
         <f t="shared" ref="Q19:R19" si="23">Q16-SUM(Q17:Q18)</f>
         <v>29.777282999999997</v>
       </c>
-      <c r="R19" s="122">
+      <c r="R19" s="120">
         <f t="shared" si="23"/>
         <v>15.517839000000004</v>
       </c>
-      <c r="S19" s="122">
+      <c r="S19" s="120">
         <f t="shared" ref="S19:Y19" si="24">S16-SUM(S17:S18)</f>
         <v>24.277938999999968</v>
       </c>
-      <c r="T19" s="122">
+      <c r="T19" s="120">
         <f t="shared" si="24"/>
         <v>36.256999999999991</v>
       </c>
-      <c r="U19" s="122">
+      <c r="U19" s="120">
         <f t="shared" si="24"/>
         <v>26.874999999999996</v>
       </c>
-      <c r="V19" s="126">
+      <c r="V19" s="124">
         <f t="shared" si="24"/>
         <v>26.332000000000008</v>
       </c>
-      <c r="W19" s="122">
+      <c r="W19" s="120">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="X19" s="122">
+      <c r="X19" s="120">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="122">
+      <c r="Y19" s="120">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
@@ -17509,58 +17534,58 @@
       <c r="B20" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="124">
+      <c r="C20" s="122">
         <v>186.842646</v>
       </c>
-      <c r="D20" s="124">
+      <c r="D20" s="122">
         <v>200.34402800000001</v>
       </c>
-      <c r="E20" s="124">
+      <c r="E20" s="122">
         <v>5.4436049999999998</v>
       </c>
-      <c r="F20" s="124">
+      <c r="F20" s="122">
         <v>5.6785269999999999</v>
       </c>
-      <c r="G20" s="125">
+      <c r="G20" s="123">
         <v>5.981795</v>
       </c>
-      <c r="H20" s="124">
+      <c r="H20" s="122">
         <f>T20</f>
         <v>36.170999999999999</v>
       </c>
       <c r="L20" s="17">
         <v>5.5568299999999997</v>
       </c>
-      <c r="M20" s="124">
+      <c r="M20" s="122">
         <v>5.6557409999999999</v>
       </c>
-      <c r="N20" s="123">
+      <c r="N20" s="121">
         <v>5.7296649999999998</v>
       </c>
-      <c r="O20" s="124">
+      <c r="O20" s="122">
         <f>F20</f>
         <v>5.6785269999999999</v>
       </c>
-      <c r="P20" s="124">
+      <c r="P20" s="122">
         <v>5.9607679999999998</v>
       </c>
-      <c r="Q20" s="124">
+      <c r="Q20" s="122">
         <v>6.0243779999999996</v>
       </c>
-      <c r="R20" s="124">
+      <c r="R20" s="122">
         <v>5.9058830000000002</v>
       </c>
-      <c r="S20" s="124">
+      <c r="S20" s="122">
         <f>G20</f>
         <v>5.981795</v>
       </c>
-      <c r="T20" s="124">
+      <c r="T20" s="122">
         <v>36.170999999999999</v>
       </c>
-      <c r="U20" s="124">
+      <c r="U20" s="122">
         <v>35.506999999999998</v>
       </c>
-      <c r="V20" s="125">
+      <c r="V20" s="123">
         <v>35.674999999999997</v>
       </c>
     </row>
@@ -17580,15 +17605,20 @@
         <f>E19/E20</f>
         <v>-6.77600064663031</v>
       </c>
-      <c r="F21" s="134">
+      <c r="F21" s="132">
         <f>F19/F20</f>
         <v>1.2505086266209531</v>
       </c>
-      <c r="G21" s="51">
+      <c r="G21" s="50">
         <f>G19/G20</f>
         <v>12.969604775823973</v>
       </c>
-      <c r="H21" s="52"/>
+      <c r="H21" s="163">
+        <v>3.27</v>
+      </c>
+      <c r="I21" s="8">
+        <v>4.2699999999999996</v>
+      </c>
       <c r="L21" s="2">
         <f t="shared" ref="L21:M21" si="25">(L19+L18)/L20</f>
         <v>0.3103470863783851</v>
@@ -17633,13 +17663,13 @@
         <f t="shared" si="27"/>
         <v>0.74761037140854969</v>
       </c>
-      <c r="W21" s="2" t="e">
-        <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X21" s="2" t="e">
-        <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+      <c r="W21" s="8">
+        <f>W22</f>
+        <v>0.98</v>
+      </c>
+      <c r="X21" s="8">
+        <f>X22</f>
+        <v>1.22</v>
       </c>
       <c r="Y21" s="2" t="e">
         <f t="shared" si="27"/>
@@ -17654,34 +17684,37 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="136">
+      <c r="G22" s="134">
         <v>6.73</v>
       </c>
-      <c r="H22" s="43">
-        <v>3.27</v>
+      <c r="H22" s="42">
+        <v>3.38</v>
       </c>
       <c r="I22" s="1">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="44">
+        <v>4.38</v>
+      </c>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43">
         <v>0.89</v>
       </c>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="139">
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="137">
         <v>0.56000000000000005</v>
       </c>
-      <c r="V22" s="140">
+      <c r="V22" s="138">
         <v>0.65</v>
       </c>
       <c r="W22" s="1">
-        <v>0.9</v>
+        <v>0.98</v>
+      </c>
+      <c r="X22" s="1">
+        <v>1.22</v>
       </c>
     </row>
     <row r="23" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17708,13 +17741,13 @@
         <f t="shared" ref="G23:I23" si="29">1-(G6)/G3</f>
         <v>0.81055306777919456</v>
       </c>
-      <c r="H23" s="38" t="e">
+      <c r="H23" s="38">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="38" t="e">
+        <v>1</v>
+      </c>
+      <c r="I23" s="38">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L23" s="38">
         <f t="shared" ref="L23:S23" si="30">1-(L6)/L3</f>
@@ -17797,13 +17830,13 @@
         <f t="shared" ref="G24:I24" si="33">G19/G3</f>
         <v>0.28614362395546977</v>
       </c>
-      <c r="H24" s="3" t="e">
+      <c r="H24" s="3">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" s="3" t="e">
+        <v>0.27219249265295214</v>
+      </c>
+      <c r="I24" s="3">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" ref="L24:Q24" si="34">L19/L3</f>
@@ -17853,85 +17886,87 @@
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="X24" s="3" t="e">
+      <c r="X24" s="3">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="3" t="e">
         <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:25" s="127" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="127" t="s">
+    <row r="25" spans="2:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128">
+      <c r="C25" s="162"/>
+      <c r="D25" s="126">
         <f>D3/C3-1</f>
         <v>0.95305337511785693</v>
       </c>
-      <c r="E25" s="129">
+      <c r="E25" s="127">
         <f>E3/D3-1</f>
         <v>9.3660696466152382E-2</v>
       </c>
-      <c r="F25" s="129">
+      <c r="F25" s="127">
         <f>F3/E3-1</f>
         <v>0.26906277250392074</v>
       </c>
-      <c r="G25" s="130">
+      <c r="G25" s="128">
         <f t="shared" ref="G25:I25" si="37">G3/F3-1</f>
         <v>0.70138919480622985</v>
       </c>
-      <c r="H25" s="129">
+      <c r="H25" s="127">
         <f t="shared" si="37"/>
-        <v>-1</v>
-      </c>
-      <c r="I25" s="129" t="e">
+        <v>0.65663517685325568</v>
+      </c>
+      <c r="I25" s="127">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="129"/>
-      <c r="M25" s="129"/>
-      <c r="N25" s="129"/>
-      <c r="O25" s="129"/>
-      <c r="P25" s="129">
+        <v>0.2601522842639592</v>
+      </c>
+      <c r="J25" s="167"/>
+      <c r="K25" s="167"/>
+      <c r="L25" s="168"/>
+      <c r="M25" s="168"/>
+      <c r="N25" s="168"/>
+      <c r="O25" s="168"/>
+      <c r="P25" s="127">
         <f t="shared" ref="P25" si="38">P3/L3-1</f>
         <v>0.3548885312214991</v>
       </c>
-      <c r="Q25" s="129">
+      <c r="Q25" s="127">
         <f t="shared" ref="Q25:V25" si="39">Q3/M3-1</f>
         <v>0.60195322154471387</v>
       </c>
-      <c r="R25" s="129">
+      <c r="R25" s="127">
         <f t="shared" si="39"/>
         <v>0.71279372070468461</v>
       </c>
-      <c r="S25" s="129">
+      <c r="S25" s="127">
         <f t="shared" si="39"/>
         <v>1.0085909474100725</v>
       </c>
-      <c r="T25" s="129">
+      <c r="T25" s="127">
         <f t="shared" si="39"/>
         <v>1.2331854093501313</v>
       </c>
-      <c r="U25" s="129">
+      <c r="U25" s="127">
         <f t="shared" si="39"/>
         <v>0.76352754106974974</v>
       </c>
-      <c r="V25" s="130">
+      <c r="V25" s="128">
         <f t="shared" si="39"/>
         <v>0.66952336948913893</v>
       </c>
-      <c r="W25" s="129">
+      <c r="W25" s="127">
         <f>W4/S3-1</f>
-        <v>0.34744325823284306</v>
-      </c>
-      <c r="X25" s="129">
+        <v>0.31242093251829073</v>
+      </c>
+      <c r="X25" s="127">
         <f t="shared" ref="X25:Y25" si="40">X4/T3-1</f>
-        <v>-1</v>
-      </c>
-      <c r="Y25" s="129">
+        <v>0.22102333384169581</v>
+      </c>
+      <c r="Y25" s="127">
         <f t="shared" si="40"/>
         <v>-1</v>
       </c>
@@ -17960,13 +17995,13 @@
         <f t="shared" ref="G26:I26" si="41">G8/G3</f>
         <v>3.5923132068781269E-2</v>
       </c>
-      <c r="H26" s="3" t="e">
+      <c r="H26" s="3">
         <f t="shared" si="41"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" s="3" t="e">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
         <f t="shared" si="41"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L26" s="3">
         <f t="shared" ref="L26:S26" si="42">L8/L3</f>
@@ -18049,13 +18084,13 @@
         <f t="shared" ref="G27:I27" si="45">G5/G3</f>
         <v>0.19092452642920654</v>
       </c>
-      <c r="H27" s="3" t="e">
+      <c r="H27" s="3">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" s="3" t="e">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
         <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L27" s="3">
         <f t="shared" ref="L27:S27" si="46">L5/L3</f>
@@ -18138,13 +18173,13 @@
         <f t="shared" ref="G28:I28" si="49">G11/G3</f>
         <v>0</v>
       </c>
-      <c r="H28" s="3" t="e">
+      <c r="H28" s="3">
         <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="3" t="e">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
         <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" ref="L28:S28" si="50">L11/L3</f>
@@ -18203,76 +18238,78 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:25" s="127" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="127" t="s">
+    <row r="29" spans="2:25" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="125" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128">
+      <c r="C29" s="126"/>
+      <c r="D29" s="126">
         <f>-(D19/C19-1)</f>
         <v>-1.2884450628390551</v>
       </c>
-      <c r="E29" s="129">
+      <c r="E29" s="127">
         <f>E19/D19-1</f>
         <v>-0.50974262673844062</v>
       </c>
-      <c r="F29" s="129">
+      <c r="F29" s="127">
         <f>F21/E21-1</f>
         <v>-1.1845496616419049</v>
       </c>
-      <c r="G29" s="130">
+      <c r="G29" s="128">
         <f t="shared" ref="G29" si="53">G21/F21-1</f>
         <v>9.3714636586471496</v>
       </c>
-      <c r="H29" s="129">
+      <c r="H29" s="127">
         <f>H22/(G21*G20/H20)-1</f>
-        <v>0.52457923708813348</v>
-      </c>
-      <c r="I29" s="129">
+        <v>0.57586477717366691</v>
+      </c>
+      <c r="I29" s="127">
         <f>I22/(H22)-1</f>
-        <v>0.30581039755351669</v>
-      </c>
-      <c r="L29" s="129"/>
-      <c r="M29" s="129"/>
-      <c r="N29" s="129"/>
-      <c r="O29" s="129"/>
-      <c r="P29" s="129">
+        <v>0.29585798816568043</v>
+      </c>
+      <c r="J29" s="167"/>
+      <c r="K29" s="167"/>
+      <c r="L29" s="168"/>
+      <c r="M29" s="168"/>
+      <c r="N29" s="168"/>
+      <c r="O29" s="168"/>
+      <c r="P29" s="127">
         <f t="shared" ref="P29" si="54">P21/L21-1</f>
         <v>3.3283284406211981</v>
       </c>
-      <c r="Q29" s="129">
+      <c r="Q29" s="127">
         <f>Q21/M21-1</f>
         <v>23.46476131398072</v>
       </c>
-      <c r="R29" s="129">
+      <c r="R29" s="127">
         <f>R21/N21-1</f>
         <v>10.577070923879727</v>
       </c>
-      <c r="S29" s="129">
+      <c r="S29" s="127">
         <f>S21/O21-1</f>
         <v>7.1928086112209204</v>
       </c>
-      <c r="T29" s="129">
+      <c r="T29" s="127">
         <f>T21/(P21*P20/T20)-1</f>
         <v>3.5165452001091522</v>
       </c>
-      <c r="U29" s="129">
+      <c r="U29" s="127">
         <f>U21/(Q21*Q20/U20)-1</f>
         <v>-7.0631250593186423E-2</v>
       </c>
-      <c r="V29" s="130">
+      <c r="V29" s="128">
         <f t="shared" ref="V29:Y29" si="55">V22/(R21*R20/U20)-1</f>
         <v>0.49418554326583353</v>
       </c>
-      <c r="W29" s="129">
-        <f t="shared" si="55"/>
-        <v>0.26571006068312664</v>
-      </c>
-      <c r="X29" s="129" t="e">
-        <f t="shared" si="55"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y29" s="129" t="e">
+      <c r="W29" s="127">
+        <f>W22/(S21*S20/V20)-1</f>
+        <v>0.37821762163273775</v>
+      </c>
+      <c r="X29" s="127">
+        <f>X22/(T21*T20/V20)-1</f>
+        <v>0.20350348412786223</v>
+      </c>
+      <c r="Y29" s="127" t="e">
         <f t="shared" si="55"/>
         <v>#DIV/0!</v>
       </c>
@@ -18281,87 +18318,87 @@
       <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="46">
         <f>C13/C3</f>
         <v>-7.3197846788253168E-2</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <f>D13/D3</f>
         <v>-4.5893036318300044E-2</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="46">
         <f>E13/E3</f>
         <v>-6.8493157557677126E-2</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="46">
         <f>F13/F3</f>
         <v>-0.10020521751030448</v>
       </c>
-      <c r="G30" s="48">
+      <c r="G30" s="47">
         <f t="shared" ref="G30:I30" si="56">G13/G3</f>
         <v>-5.075702466463336E-2</v>
       </c>
-      <c r="H30" s="47" t="e">
+      <c r="H30" s="46">
         <f t="shared" si="56"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I30" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="I30" s="46">
         <f t="shared" si="56"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="47">
+        <v>0</v>
+      </c>
+      <c r="L30" s="46">
         <f t="shared" ref="L30:S30" si="57">L13/L3</f>
         <v>-9.7395812949690505E-2</v>
       </c>
-      <c r="M30" s="47">
+      <c r="M30" s="46">
         <f t="shared" si="57"/>
         <v>-0.11258468475211493</v>
       </c>
-      <c r="N30" s="47">
+      <c r="N30" s="46">
         <f t="shared" si="57"/>
         <v>-0.1014405447666855</v>
       </c>
-      <c r="O30" s="47">
+      <c r="O30" s="46">
         <f t="shared" si="57"/>
         <v>-9.232091670036538E-2</v>
       </c>
-      <c r="P30" s="47">
+      <c r="P30" s="46">
         <f t="shared" si="57"/>
         <v>-8.6878686170398234E-2</v>
       </c>
-      <c r="Q30" s="47">
+      <c r="Q30" s="46">
         <f>Q13/Q3</f>
         <v>-5.2013770959220725E-2</v>
       </c>
-      <c r="R30" s="47">
+      <c r="R30" s="46">
         <f>R13/R3</f>
         <v>-4.7571581514890195E-2</v>
       </c>
-      <c r="S30" s="47">
+      <c r="S30" s="46">
         <f t="shared" si="57"/>
         <v>-3.5033239648612068E-2</v>
       </c>
-      <c r="T30" s="47">
+      <c r="T30" s="46">
         <f t="shared" ref="T30:U30" si="58">T13/T3</f>
         <v>-2.7775659600427025E-2</v>
       </c>
-      <c r="U30" s="47">
+      <c r="U30" s="46">
         <f t="shared" si="58"/>
         <v>-3.5470405868168832E-2</v>
       </c>
-      <c r="V30" s="48">
+      <c r="V30" s="47">
         <f t="shared" ref="V30:Y30" si="59">V13/V3</f>
         <v>-3.3588479057501966E-2</v>
       </c>
-      <c r="W30" s="47" t="e">
+      <c r="W30" s="46" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X30" s="47" t="e">
+      <c r="X30" s="46" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y30" s="47" t="e">
+      <c r="Y30" s="46" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18370,87 +18407,87 @@
       <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="49">
+      <c r="C31" s="48">
         <f t="shared" ref="C31:F31" si="60">-C13/C12</f>
         <v>-0.1541124283771651</v>
       </c>
-      <c r="D31" s="49">
+      <c r="D31" s="48">
         <f t="shared" si="60"/>
         <v>-7.671907679879103E-2</v>
       </c>
-      <c r="E31" s="49">
+      <c r="E31" s="48">
         <f t="shared" si="60"/>
         <v>-0.30247355291202405</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F31" s="46">
         <f t="shared" si="60"/>
         <v>0.71928340393491097</v>
       </c>
-      <c r="G31" s="48">
+      <c r="G31" s="47">
         <f t="shared" ref="G31:I31" si="61">-G13/G12</f>
         <v>0.16732385305731867</v>
       </c>
-      <c r="H31" s="47" t="e">
+      <c r="H31" s="46">
         <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I31" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="I31" s="46">
         <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="49">
+        <v>0</v>
+      </c>
+      <c r="L31" s="48">
         <f t="shared" ref="L31:S31" si="62">-L13/L12</f>
         <v>0.62307933440481045</v>
       </c>
-      <c r="M31" s="49">
+      <c r="M31" s="48">
         <f t="shared" si="62"/>
         <v>1.0452144147237079</v>
       </c>
-      <c r="N31" s="49">
+      <c r="N31" s="48">
         <f t="shared" si="62"/>
         <v>0.77447766201940493</v>
       </c>
-      <c r="O31" s="49">
+      <c r="O31" s="48">
         <f t="shared" si="62"/>
         <v>0.58880572040137491</v>
       </c>
-      <c r="P31" s="49">
+      <c r="P31" s="48">
         <f t="shared" si="62"/>
         <v>0.2950157709005724</v>
       </c>
-      <c r="Q31" s="47">
+      <c r="Q31" s="46">
         <f>-Q13/Q12</f>
         <v>0.1743258132936672</v>
       </c>
-      <c r="R31" s="47">
+      <c r="R31" s="46">
         <f t="shared" si="62"/>
         <v>0.15968382966580907</v>
       </c>
-      <c r="S31" s="47">
+      <c r="S31" s="46">
         <f t="shared" si="62"/>
         <v>0.11146848377981249</v>
       </c>
-      <c r="T31" s="47">
+      <c r="T31" s="46">
         <f t="shared" ref="T31:U31" si="63">-T13/T12</f>
         <v>5.8402645555666911E-2</v>
       </c>
-      <c r="U31" s="47">
+      <c r="U31" s="46">
         <f t="shared" si="63"/>
         <v>9.7018234218256394E-2</v>
       </c>
-      <c r="V31" s="48">
+      <c r="V31" s="47">
         <f t="shared" ref="V31:Y31" si="64">-V13/V12</f>
         <v>0.11031748263547142</v>
       </c>
-      <c r="W31" s="47" t="e">
+      <c r="W31" s="46" t="e">
         <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X31" s="47" t="e">
+      <c r="X31" s="46" t="e">
         <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y31" s="47" t="e">
+      <c r="Y31" s="46" t="e">
         <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
@@ -18567,7 +18604,7 @@
       </c>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
-      <c r="N35" s="124">
+      <c r="N35" s="122">
         <v>65.150279999999995</v>
       </c>
       <c r="O35" s="9">
@@ -18618,7 +18655,7 @@
       </c>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
-      <c r="N36" s="124">
+      <c r="N36" s="122">
         <v>1.5804180000000001</v>
       </c>
       <c r="O36" s="9">
@@ -18669,7 +18706,7 @@
       </c>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
-      <c r="N37" s="124">
+      <c r="N37" s="122">
         <v>111.146024</v>
       </c>
       <c r="O37" s="9">
@@ -18716,7 +18753,7 @@
       </c>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="N38" s="124">
+      <c r="N38" s="122">
         <v>-8.5979419999999998</v>
       </c>
       <c r="O38" s="9">
@@ -20119,15 +20156,15 @@
       <c r="B64" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="135"/>
-      <c r="G64" s="137">
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="133"/>
+      <c r="G64" s="135">
         <f>G19/G62</f>
         <v>1.0892481418664739</v>
       </c>
-      <c r="H64" s="131" t="e">
+      <c r="H64" s="129" t="e">
         <f>H19/H62</f>
         <v>#DIV/0!</v>
       </c>
@@ -20144,7 +20181,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="P37:V37">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -20152,6 +20189,42 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P25:Y25">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:I25">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:I29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -20177,46 +20250,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="138">
+      <c r="B1" s="136">
         <v>45413</v>
       </c>
-      <c r="C1" s="138">
+      <c r="C1" s="136">
         <v>45444</v>
       </c>
-      <c r="D1" s="138">
+      <c r="D1" s="136">
         <v>45474</v>
       </c>
-      <c r="E1" s="138">
+      <c r="E1" s="136">
         <v>45505</v>
       </c>
-      <c r="F1" s="138">
+      <c r="F1" s="136">
         <v>45536</v>
       </c>
-      <c r="G1" s="138">
+      <c r="G1" s="136">
         <v>45566</v>
       </c>
-      <c r="H1" s="138">
+      <c r="H1" s="136">
         <v>45597</v>
       </c>
-      <c r="I1" s="138">
+      <c r="I1" s="136">
         <v>45627</v>
       </c>
-      <c r="J1" s="138">
+      <c r="J1" s="136">
         <v>45658</v>
       </c>
-      <c r="K1" s="138">
+      <c r="K1" s="136">
         <v>45689</v>
       </c>
-      <c r="L1" s="138">
+      <c r="L1" s="136">
         <v>45717</v>
       </c>
-      <c r="M1" s="138">
+      <c r="M1" s="136">
         <v>45748</v>
       </c>
-      <c r="N1" s="138">
+      <c r="N1" s="136">
         <v>45778</v>
       </c>
-      <c r="O1" s="138">
+      <c r="O1" s="136">
         <v>45809</v>
       </c>
     </row>
@@ -20495,41 +20568,41 @@
       <c r="A5" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="133">
+      <c r="B5" s="131">
         <v>0.93799999999999994</v>
       </c>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133">
+      <c r="C5" s="131"/>
+      <c r="D5" s="131">
         <v>0.94399999999999995</v>
       </c>
-      <c r="E5" s="133">
+      <c r="E5" s="131">
         <v>0.94699999999999995</v>
       </c>
-      <c r="F5" s="133">
+      <c r="F5" s="131">
         <v>0.95699999999999996</v>
       </c>
-      <c r="G5" s="133">
+      <c r="G5" s="131">
         <v>0.95299999999999996</v>
       </c>
-      <c r="H5" s="133">
+      <c r="H5" s="131">
         <v>0.95599999999999996</v>
       </c>
-      <c r="I5" s="133">
+      <c r="I5" s="131">
         <v>0.95499999999999996</v>
       </c>
-      <c r="J5" s="133">
+      <c r="J5" s="131">
         <v>0.95699999999999996</v>
       </c>
-      <c r="K5" s="133">
+      <c r="K5" s="131">
         <v>0.96</v>
       </c>
-      <c r="L5" s="133">
+      <c r="L5" s="131">
         <v>0.96199999999999997</v>
       </c>
-      <c r="M5" s="133">
+      <c r="M5" s="131">
         <v>0.96399999999999997</v>
       </c>
-      <c r="N5" s="133">
+      <c r="N5" s="131">
         <v>0.96599999999999997</v>
       </c>
     </row>
@@ -20633,43 +20706,43 @@
       <c r="A9" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="132"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132">
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130">
         <f>F2/B2-1</f>
         <v>1.3863636363636362</v>
       </c>
-      <c r="G9" s="132" t="e">
+      <c r="G9" s="130" t="e">
         <f t="shared" ref="G9:I9" si="0">G2/C2-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="132">
+      <c r="H9" s="130">
         <f>H2/D2-1</f>
         <v>1.612676056338028</v>
       </c>
-      <c r="I9" s="132">
+      <c r="I9" s="130">
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
-      <c r="J9" s="132">
+      <c r="J9" s="130">
         <f t="shared" ref="J9" si="1">J2/F2-1</f>
         <v>1.519047619047619</v>
       </c>
-      <c r="K9" s="132">
+      <c r="K9" s="130">
         <f t="shared" ref="K9" si="2">K2/G2-1</f>
         <v>1.3029315960912053</v>
       </c>
-      <c r="L9" s="132">
+      <c r="L9" s="130">
         <f t="shared" ref="L9:N9" si="3">L2/H2-1</f>
         <v>0.77358490566037741</v>
       </c>
-      <c r="M9" s="132">
+      <c r="M9" s="130">
         <f t="shared" si="3"/>
         <v>0.61904761904761907</v>
       </c>
-      <c r="N9" s="132">
+      <c r="N9" s="130">
         <f t="shared" si="3"/>
         <v>0.48204158790170126</v>
       </c>
@@ -20678,43 +20751,43 @@
       <c r="A10" t="s">
         <v>190</v>
       </c>
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132">
+      <c r="B10" s="130"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130">
         <f>F7/B7-1</f>
         <v>0.24891067538126355</v>
       </c>
-      <c r="G10" s="132" t="e">
+      <c r="G10" s="130" t="e">
         <f t="shared" ref="G10:I10" si="4">G7/C7-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="132">
+      <c r="H10" s="130">
         <f t="shared" si="4"/>
         <v>0.4591309632330598</v>
       </c>
-      <c r="I10" s="132">
+      <c r="I10" s="130">
         <f t="shared" si="4"/>
         <v>0.47308699447192315</v>
       </c>
-      <c r="J10" s="132">
+      <c r="J10" s="130">
         <f t="shared" ref="J10" si="5">J7/F7-1</f>
         <v>0.36153510684692547</v>
       </c>
-      <c r="K10" s="132">
+      <c r="K10" s="130">
         <f t="shared" ref="K10" si="6">K7/G7-1</f>
         <v>0.33761342235918512</v>
       </c>
-      <c r="L10" s="132">
+      <c r="L10" s="130">
         <f t="shared" ref="L10:N10" si="7">L7/H7-1</f>
         <v>0.52269887546855487</v>
       </c>
-      <c r="M10" s="132">
+      <c r="M10" s="130">
         <f t="shared" si="7"/>
         <v>0.62630851273948251</v>
       </c>
-      <c r="N10" s="132">
+      <c r="N10" s="130">
         <f t="shared" si="7"/>
         <v>0.52674567584881493</v>
       </c>
@@ -20749,17 +20822,17 @@
       <c r="A14" t="s">
         <v>212</v>
       </c>
-      <c r="J14" s="141"/>
-      <c r="K14" s="141"/>
-      <c r="L14" s="141">
+      <c r="J14" s="139"/>
+      <c r="K14" s="139"/>
+      <c r="L14" s="139">
         <f>L13/H13-1</f>
         <v>0.64136391313172325</v>
       </c>
-      <c r="M14" s="141">
+      <c r="M14" s="139">
         <f>M13/I13-1</f>
         <v>0.74182638105975185</v>
       </c>
-      <c r="N14" s="141">
+      <c r="N14" s="139">
         <f>N13/J13-1</f>
         <v>0.58705864524928009</v>
       </c>
@@ -20768,31 +20841,31 @@
       <c r="A16" t="s">
         <v>213</v>
       </c>
-      <c r="H16" s="141">
+      <c r="H16" s="139">
         <f>Model!P3/KPIs!H13</f>
         <v>9.5349368784250058E-2</v>
       </c>
-      <c r="I16" s="141">
+      <c r="I16" s="139">
         <f>Model!Q3/KPIs!I13</f>
         <v>0.10516442127019916</v>
       </c>
-      <c r="J16" s="141">
+      <c r="J16" s="139">
         <f>Model!R3/KPIs!J13</f>
         <v>0.10601256402485225</v>
       </c>
-      <c r="K16" s="141">
+      <c r="K16" s="139">
         <f>Model!S3/KPIs!K13</f>
         <v>0.1148270516717325</v>
       </c>
-      <c r="L16" s="141">
+      <c r="L16" s="139">
         <f>Model!T3/KPIs!L13</f>
         <v>0.12972919500432795</v>
       </c>
-      <c r="M16" s="141">
+      <c r="M16" s="139">
         <f>Model!U3/KPIs!M13</f>
         <v>0.10647464940668824</v>
       </c>
-      <c r="N16" s="141">
+      <c r="N16" s="139">
         <f>Model!V3/KPIs!N13</f>
         <v>0.11152105413921513</v>
       </c>
@@ -20857,13 +20930,13 @@
       <c r="A21" t="s">
         <v>215</v>
       </c>
-      <c r="B21" s="161">
+      <c r="B21" s="140">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="C21" s="161">
+      <c r="C21" s="140">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D21" s="161">
+      <c r="D21" s="140">
         <v>2.18E-2</v>
       </c>
       <c r="E21" s="17">
@@ -20890,18 +20963,18 @@
         <f>E21/G21</f>
         <v>46.454545454545453</v>
       </c>
-      <c r="N21" s="132">
+      <c r="N21" s="130">
         <v>1</v>
       </c>
-      <c r="P21" s="132">
+      <c r="P21" s="130">
         <f>J21/I21-1</f>
         <v>0.28774928774928776</v>
       </c>
-      <c r="R21" s="162">
+      <c r="R21" s="141">
         <f>11567/I21</f>
         <v>3.2954415954415954</v>
       </c>
-      <c r="S21" s="162">
+      <c r="S21" s="141">
         <f>11567/J21</f>
         <v>2.5590707964601771</v>
       </c>
@@ -20910,7 +20983,7 @@
       <c r="A22" t="s">
         <v>222</v>
       </c>
-      <c r="C22" s="161">
+      <c r="C22" s="140">
         <v>2.4E-2</v>
       </c>
       <c r="E22">
@@ -20937,19 +21010,19 @@
         <f t="shared" ref="L22:L24" si="9">E22/G22</f>
         <v>17.783289817232376</v>
       </c>
-      <c r="N22" s="132">
+      <c r="N22" s="130">
         <f t="shared" ref="N22:N24" si="10">G22/F22-1</f>
         <v>0.23151125401929273</v>
       </c>
-      <c r="P22" s="132">
+      <c r="P22" s="130">
         <f t="shared" ref="P22:P24" si="11">J22/I22-1</f>
         <v>0.24019607843137258</v>
       </c>
-      <c r="R22" s="162">
+      <c r="R22" s="141">
         <f>22481/I22</f>
         <v>5.5100490196078429</v>
       </c>
-      <c r="S22" s="162">
+      <c r="S22" s="141">
         <f>22481/J22</f>
         <v>4.4428853754940709</v>
       </c>
@@ -20982,19 +21055,19 @@
         <f t="shared" si="9"/>
         <v>15.456621004566211</v>
       </c>
-      <c r="N23" s="132">
+      <c r="N23" s="130">
         <f t="shared" si="10"/>
         <v>0.29585798816568043</v>
       </c>
-      <c r="P23" s="132">
+      <c r="P23" s="130">
         <f t="shared" si="11"/>
         <v>0.2601522842639592</v>
       </c>
-      <c r="R23" s="162">
+      <c r="R23" s="141">
         <f>2312/I23</f>
         <v>5.1473862320776558</v>
       </c>
-      <c r="S23" s="162">
+      <c r="S23" s="141">
         <f>2312/J23</f>
         <v>4.0847334852741115</v>
       </c>
@@ -21027,19 +21100,19 @@
         <f t="shared" si="9"/>
         <v>10.494845360824742</v>
       </c>
-      <c r="N24" s="132">
+      <c r="N24" s="130">
         <f t="shared" si="10"/>
         <v>8.7850467289719791E-2</v>
       </c>
-      <c r="P24" s="132">
+      <c r="P24" s="130">
         <f t="shared" si="11"/>
         <v>5.9723889555822307E-2</v>
       </c>
-      <c r="R24" s="162">
+      <c r="R24" s="141">
         <f>58393/I24</f>
         <v>1.7524909963985593</v>
       </c>
-      <c r="S24" s="162">
+      <c r="S24" s="141">
         <f>58393/J24</f>
         <v>1.6537241574624753</v>
       </c>
@@ -29448,34 +29521,34 @@
         <f>C2/C3-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="61"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" t="e">
         <f t="shared" ref="D3:D66" si="0">C3/C4-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="64" t="s">
+      <c r="J3" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="65" t="s">
+      <c r="L3" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="66" t="s">
+      <c r="M3" s="64" t="s">
         <v>90</v>
       </c>
     </row>
@@ -29484,27 +29557,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H4" s="67" t="e">
+      <c r="H4" s="65" t="e">
         <f>$I$19-3*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="68" t="e">
+      <c r="I4" s="66" t="e">
         <f>H4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="69">
+      <c r="J4" s="67">
         <f>COUNTIF(D:D,"&lt;="&amp;H4)</f>
         <v>67</v>
       </c>
-      <c r="K4" s="69" t="e">
+      <c r="K4" s="67" t="e">
         <f>"Less than "&amp;TEXT(H4,"0,00%")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L4" s="70" t="e">
+      <c r="L4" s="68" t="e">
         <f>J4/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M4" s="71" t="e">
+      <c r="M4" s="69" t="e">
         <f>L4</f>
         <v>#DIV/0!</v>
       </c>
@@ -29514,27 +29587,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="72" t="e">
+      <c r="H5" s="70" t="e">
         <f>$I$19-2.4*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="73" t="e">
+      <c r="I5" s="71" t="e">
         <f>H5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="74">
+      <c r="J5" s="72">
         <f>COUNTIFS(D:D,"&lt;="&amp;H5,D:D,"&gt;"&amp;H4)</f>
         <v>67</v>
       </c>
-      <c r="K5" s="75" t="e">
+      <c r="K5" s="73" t="e">
         <f t="shared" ref="K5:K14" si="1">TEXT(H4,"0,00%")&amp;" to "&amp;TEXT(H5,"0,00%")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L5" s="76" t="e">
+      <c r="L5" s="74" t="e">
         <f>J5/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M5" s="77" t="e">
+      <c r="M5" s="75" t="e">
         <f>M4+L5</f>
         <v>#DIV/0!</v>
       </c>
@@ -29544,27 +29617,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="72" t="e">
+      <c r="H6" s="70" t="e">
         <f>$I$19-1.8*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="73" t="e">
+      <c r="I6" s="71" t="e">
         <f t="shared" ref="I6:I14" si="2">H6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="74">
+      <c r="J6" s="72">
         <f t="shared" ref="J6:J14" si="3">COUNTIFS(D:D,"&lt;="&amp;H6,D:D,"&gt;"&amp;H5)</f>
         <v>67</v>
       </c>
-      <c r="K6" s="75" t="e">
+      <c r="K6" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L6" s="76" t="e">
+      <c r="L6" s="74" t="e">
         <f t="shared" ref="L6:L15" si="4">J6/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="77" t="e">
+      <c r="M6" s="75" t="e">
         <f t="shared" ref="M6:M15" si="5">M5+L6</f>
         <v>#DIV/0!</v>
       </c>
@@ -29574,27 +29647,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="72" t="e">
+      <c r="H7" s="70" t="e">
         <f>$I$19-1.2*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="73" t="e">
+      <c r="I7" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="74">
+      <c r="J7" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K7" s="75" t="e">
+      <c r="K7" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L7" s="76" t="e">
+      <c r="L7" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M7" s="77" t="e">
+      <c r="M7" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29604,27 +29677,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="72" t="e">
+      <c r="H8" s="70" t="e">
         <f>$I$19-0.6*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="73" t="e">
+      <c r="I8" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="74">
+      <c r="J8" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K8" s="75" t="e">
+      <c r="K8" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L8" s="76" t="e">
+      <c r="L8" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="77" t="e">
+      <c r="M8" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29634,27 +29707,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="72" t="e">
+      <c r="H9" s="70" t="e">
         <f>$I$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="73" t="e">
+      <c r="I9" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="74">
+      <c r="J9" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K9" s="75" t="e">
+      <c r="K9" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L9" s="76" t="e">
+      <c r="L9" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M9" s="77" t="e">
+      <c r="M9" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29664,27 +29737,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="72" t="e">
+      <c r="H10" s="70" t="e">
         <f>$I$19+0.6*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="73" t="e">
+      <c r="I10" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="74">
+      <c r="J10" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K10" s="75" t="e">
+      <c r="K10" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L10" s="76" t="e">
+      <c r="L10" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="77" t="e">
+      <c r="M10" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29694,27 +29767,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H11" s="72" t="e">
+      <c r="H11" s="70" t="e">
         <f>$I$19+1.2*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="73" t="e">
+      <c r="I11" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="74">
+      <c r="J11" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K11" s="75" t="e">
+      <c r="K11" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L11" s="76" t="e">
+      <c r="L11" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="77" t="e">
+      <c r="M11" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29724,27 +29797,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H12" s="72" t="e">
+      <c r="H12" s="70" t="e">
         <f>$I$19+1.8*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="73" t="e">
+      <c r="I12" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="74">
+      <c r="J12" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K12" s="75" t="e">
+      <c r="K12" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L12" s="76" t="e">
+      <c r="L12" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M12" s="77" t="e">
+      <c r="M12" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29754,27 +29827,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H13" s="72" t="e">
+      <c r="H13" s="70" t="e">
         <f>$I$19+2.4*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="73" t="e">
+      <c r="I13" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="74">
+      <c r="J13" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K13" s="75" t="e">
+      <c r="K13" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L13" s="76" t="e">
+      <c r="L13" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="77" t="e">
+      <c r="M13" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29784,27 +29857,27 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H14" s="72" t="e">
+      <c r="H14" s="70" t="e">
         <f>$I$19+3*$I$23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I14" s="73" t="e">
+      <c r="I14" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="74">
+      <c r="J14" s="72">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="K14" s="75" t="e">
+      <c r="K14" s="73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L14" s="76" t="e">
+      <c r="L14" s="74" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M14" s="77" t="e">
+      <c r="M14" s="75" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29814,23 +29887,23 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79" t="s">
+      <c r="H15" s="76"/>
+      <c r="I15" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="79">
+      <c r="J15" s="77">
         <f>COUNTIF(D:D,"&gt;"&amp;H14)</f>
         <v>67</v>
       </c>
-      <c r="K15" s="79" t="e">
+      <c r="K15" s="77" t="e">
         <f>"Greater than "&amp;TEXT(H14,"0,00%")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L15" s="80" t="e">
+      <c r="L15" s="78" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="80" t="e">
+      <c r="M15" s="78" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -29840,8 +29913,8 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="81"/>
-      <c r="M16" s="82"/>
+      <c r="H16" s="79"/>
+      <c r="M16" s="80"/>
     </row>
     <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" t="e">
@@ -29852,7 +29925,7 @@
         <v>122</v>
       </c>
       <c r="I17" s="155"/>
-      <c r="M17" s="82"/>
+      <c r="M17" s="80"/>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" t="e">
@@ -29861,328 +29934,328 @@
       </c>
       <c r="H18" s="156"/>
       <c r="I18" s="157"/>
-      <c r="M18" s="82"/>
+      <c r="M18" s="80"/>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H19" s="83" t="s">
+      <c r="H19" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="119" t="e">
+      <c r="I19" s="117" t="e">
         <f>AVERAGE(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M19" s="82"/>
+      <c r="M19" s="80"/>
     </row>
     <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D20" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="119" t="e">
+      <c r="I20" s="117" t="e">
         <f>_xlfn.STDEV.S(D:D)/SQRT(COUNT(D:D))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M20" s="82"/>
+      <c r="M20" s="80"/>
     </row>
     <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D21" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H21" s="83" t="s">
+      <c r="H21" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="119" t="e">
+      <c r="I21" s="117" t="e">
         <f>MEDIAN(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M21" s="82"/>
+      <c r="M21" s="80"/>
     </row>
     <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H22" s="83" t="s">
+      <c r="H22" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="I22" s="119" t="e">
+      <c r="I22" s="117" t="e">
         <f>MODE(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M22" s="82"/>
+      <c r="M22" s="80"/>
     </row>
     <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D23" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H23" s="83" t="s">
+      <c r="H23" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="I23" s="119" t="e">
+      <c r="I23" s="117" t="e">
         <f>_xlfn.STDEV.S(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M23" s="82"/>
+      <c r="M23" s="80"/>
     </row>
     <row r="24" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D24" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H24" s="83" t="s">
+      <c r="H24" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="I24" s="119" t="e">
+      <c r="I24" s="117" t="e">
         <f>_xlfn.VAR.S(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M24" s="82"/>
+      <c r="M24" s="80"/>
     </row>
     <row r="25" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="I25" s="120" t="e">
+      <c r="I25" s="118" t="e">
         <f>KURT(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M25" s="82"/>
+      <c r="M25" s="80"/>
     </row>
     <row r="26" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D26" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H26" s="83" t="s">
+      <c r="H26" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="120" t="e">
+      <c r="I26" s="118" t="e">
         <f>SKEW(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M26" s="82"/>
+      <c r="M26" s="80"/>
     </row>
     <row r="27" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H27" s="83" t="s">
+      <c r="H27" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="119" t="e">
+      <c r="I27" s="117" t="e">
         <f>I29-I28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M27" s="82"/>
+      <c r="M27" s="80"/>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D28" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H28" s="83" t="s">
+      <c r="H28" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="I28" s="119" t="e">
+      <c r="I28" s="117" t="e">
         <f>MIN(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M28" s="82"/>
+      <c r="M28" s="80"/>
     </row>
     <row r="29" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D29" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="83" t="s">
+      <c r="H29" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="I29" s="119" t="e">
+      <c r="I29" s="117" t="e">
         <f>MAX(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M29" s="82"/>
+      <c r="M29" s="80"/>
     </row>
     <row r="30" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="83" t="s">
+      <c r="H30" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="I30" s="120" t="e">
+      <c r="I30" s="118" t="e">
         <f>SUM(D:D)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M30" s="82"/>
+      <c r="M30" s="80"/>
     </row>
     <row r="31" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H31" s="84" t="s">
+      <c r="H31" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="I31" s="61">
+      <c r="I31" s="59">
         <f>COUNT(D:D)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="82"/>
+      <c r="M31" s="80"/>
     </row>
     <row r="32" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H32" s="86"/>
-      <c r="M32" s="82"/>
+      <c r="H32" s="84"/>
+      <c r="M32" s="80"/>
     </row>
     <row r="33" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D33" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H33" s="87"/>
-      <c r="I33" s="88" t="s">
+      <c r="H33" s="85"/>
+      <c r="I33" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="J33" s="88" t="s">
+      <c r="J33" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="K33" s="88" t="s">
+      <c r="K33" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="L33" s="89" t="s">
+      <c r="L33" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="M33" s="82"/>
+      <c r="M33" s="80"/>
     </row>
     <row r="34" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H34" s="90" t="s">
+      <c r="H34" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="I34" s="76" t="e">
+      <c r="I34" s="74" t="e">
         <f>AVERAGEIF(D:D,"&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J34" s="74">
+      <c r="J34" s="72">
         <f>COUNTIF(D:D,"&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="K34" s="76" t="e">
+      <c r="K34" s="74" t="e">
         <f>J34/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L34" s="77" t="e">
+      <c r="L34" s="75" t="e">
         <f>K34*I34</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M34" s="82"/>
+      <c r="M34" s="80"/>
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="90" t="s">
+      <c r="H35" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="76" t="e">
+      <c r="I35" s="74" t="e">
         <f>AVERAGEIF(D:D,"&lt;0")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J35" s="74">
+      <c r="J35" s="72">
         <f>COUNTIF(D:D,"&lt;0")</f>
         <v>0</v>
       </c>
-      <c r="K35" s="76" t="e">
+      <c r="K35" s="74" t="e">
         <f>J35/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="77" t="e">
+      <c r="L35" s="75" t="e">
         <f t="shared" ref="L35:L36" si="6">K35*I35</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M35" s="82"/>
+      <c r="M35" s="80"/>
     </row>
     <row r="36" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H36" s="91" t="s">
+      <c r="H36" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="I36" s="79">
+      <c r="I36" s="77">
         <v>0</v>
       </c>
-      <c r="J36" s="79">
+      <c r="J36" s="77">
         <f>COUNTIF(D:D,"0")</f>
         <v>0</v>
       </c>
-      <c r="K36" s="92" t="e">
+      <c r="K36" s="90" t="e">
         <f>J36/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="80" t="e">
+      <c r="L36" s="78" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M36" s="82"/>
+      <c r="M36" s="80"/>
     </row>
     <row r="37" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="86"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
-      <c r="K37" s="93"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="82"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="91"/>
+      <c r="K37" s="91"/>
+      <c r="L37" s="91"/>
+      <c r="M37" s="80"/>
     </row>
     <row r="38" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="67" t="s">
+      <c r="H38" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="I38" s="88" t="s">
+      <c r="I38" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="J38" s="88" t="s">
+      <c r="J38" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="K38" s="88" t="s">
+      <c r="K38" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="L38" s="88" t="s">
+      <c r="L38" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="M38" s="89" t="s">
+      <c r="M38" s="87" t="s">
         <v>115</v>
       </c>
     </row>
@@ -30191,26 +30264,26 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="94">
+      <c r="H39" s="92">
         <v>1</v>
       </c>
-      <c r="I39" s="76" t="e">
+      <c r="I39" s="74" t="e">
         <f>$I$19+($H39*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J39" s="76" t="e">
+      <c r="J39" s="74" t="e">
         <f>$I$19-($H39*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K39" s="74">
+      <c r="K39" s="72">
         <f>COUNTIFS(D:D,"&lt;"&amp;I39,D:D,"&gt;"&amp;J39)</f>
         <v>67</v>
       </c>
-      <c r="L39" s="76" t="e">
+      <c r="L39" s="74" t="e">
         <f>K39/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M39" s="77">
+      <c r="M39" s="75">
         <v>0.68269999999999997</v>
       </c>
     </row>
@@ -30219,26 +30292,26 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H40" s="94">
+      <c r="H40" s="92">
         <v>2</v>
       </c>
-      <c r="I40" s="76" t="e">
+      <c r="I40" s="74" t="e">
         <f>$I$19+($H40*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J40" s="76" t="e">
+      <c r="J40" s="74" t="e">
         <f>$I$19-($H40*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K40" s="74">
+      <c r="K40" s="72">
         <f>COUNTIFS(D:D,"&lt;"&amp;I40,D:D,"&gt;"&amp;J40)</f>
         <v>67</v>
       </c>
-      <c r="L40" s="76" t="e">
+      <c r="L40" s="74" t="e">
         <f>K40/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M40" s="77">
+      <c r="M40" s="75">
         <v>0.95450000000000002</v>
       </c>
     </row>
@@ -30247,26 +30320,26 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="94">
+      <c r="H41" s="92">
         <v>3</v>
       </c>
-      <c r="I41" s="76" t="e">
+      <c r="I41" s="74" t="e">
         <f>$I$19+($H41*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="76" t="e">
+      <c r="J41" s="74" t="e">
         <f>$I$19-($H41*$I$23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K41" s="74">
+      <c r="K41" s="72">
         <f>COUNTIFS(D:D,"&lt;"&amp;I41,D:D,"&gt;"&amp;J41)</f>
         <v>67</v>
       </c>
-      <c r="L41" s="76" t="e">
+      <c r="L41" s="74" t="e">
         <f>K41/$I$31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M41" s="95">
+      <c r="M41" s="93">
         <v>0.99729999999999996</v>
       </c>
     </row>
@@ -30275,8 +30348,8 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H42" s="72"/>
-      <c r="M42" s="95"/>
+      <c r="H42" s="70"/>
+      <c r="M42" s="93"/>
     </row>
     <row r="43" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" t="e">
@@ -30297,24 +30370,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H44" s="96">
+      <c r="H44" s="94">
         <v>0.01</v>
       </c>
-      <c r="I44" s="97" t="e">
+      <c r="I44" s="95" t="e">
         <f t="shared" ref="I44:I58" si="7">_xlfn.PERCENTILE.INC(D:D,H44)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J44" s="98">
+      <c r="J44" s="96">
         <v>0.2</v>
       </c>
-      <c r="K44" s="97" t="e">
+      <c r="K44" s="95" t="e">
         <f t="shared" ref="K44:K56" si="8">_xlfn.PERCENTILE.INC(D:D,J44)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L44" s="98">
+      <c r="L44" s="96">
         <v>0.85</v>
       </c>
-      <c r="M44" s="99" t="e">
+      <c r="M44" s="97" t="e">
         <f t="shared" ref="M44:M58" si="9">_xlfn.PERCENTILE.INC(D:D,L44)</f>
         <v>#DIV/0!</v>
       </c>
@@ -30324,24 +30397,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H45" s="100">
+      <c r="H45" s="98">
         <v>0.02</v>
       </c>
-      <c r="I45" s="101" t="e">
+      <c r="I45" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J45" s="102">
+      <c r="J45" s="100">
         <v>0.25</v>
       </c>
-      <c r="K45" s="101" t="e">
+      <c r="K45" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L45" s="102">
+      <c r="L45" s="100">
         <v>0.86</v>
       </c>
-      <c r="M45" s="103" t="e">
+      <c r="M45" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30351,24 +30424,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H46" s="100">
+      <c r="H46" s="98">
         <v>0.03</v>
       </c>
-      <c r="I46" s="101" t="e">
+      <c r="I46" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J46" s="102">
+      <c r="J46" s="100">
         <v>0.3</v>
       </c>
-      <c r="K46" s="101" t="e">
+      <c r="K46" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L46" s="102">
+      <c r="L46" s="100">
         <v>0.87</v>
       </c>
-      <c r="M46" s="103" t="e">
+      <c r="M46" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30378,24 +30451,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H47" s="100">
+      <c r="H47" s="98">
         <v>0.04</v>
       </c>
-      <c r="I47" s="101" t="e">
+      <c r="I47" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J47" s="102">
+      <c r="J47" s="100">
         <v>0.35</v>
       </c>
-      <c r="K47" s="101" t="e">
+      <c r="K47" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L47" s="102">
+      <c r="L47" s="100">
         <v>0.88</v>
       </c>
-      <c r="M47" s="103" t="e">
+      <c r="M47" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30405,24 +30478,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H48" s="100">
+      <c r="H48" s="98">
         <v>0.05</v>
       </c>
-      <c r="I48" s="101" t="e">
+      <c r="I48" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J48" s="102">
+      <c r="J48" s="100">
         <v>0.4</v>
       </c>
-      <c r="K48" s="101" t="e">
+      <c r="K48" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L48" s="102">
+      <c r="L48" s="100">
         <v>0.89</v>
       </c>
-      <c r="M48" s="103" t="e">
+      <c r="M48" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30432,24 +30505,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H49" s="100">
+      <c r="H49" s="98">
         <v>0.06</v>
       </c>
-      <c r="I49" s="101" t="e">
+      <c r="I49" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J49" s="102">
+      <c r="J49" s="100">
         <v>0.45</v>
       </c>
-      <c r="K49" s="101" t="e">
+      <c r="K49" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L49" s="102">
+      <c r="L49" s="100">
         <v>0.9</v>
       </c>
-      <c r="M49" s="103" t="e">
+      <c r="M49" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30459,24 +30532,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H50" s="100">
+      <c r="H50" s="98">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I50" s="101" t="e">
+      <c r="I50" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J50" s="102">
+      <c r="J50" s="100">
         <v>0.5</v>
       </c>
-      <c r="K50" s="101" t="e">
+      <c r="K50" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L50" s="102">
+      <c r="L50" s="100">
         <v>0.91</v>
       </c>
-      <c r="M50" s="103" t="e">
+      <c r="M50" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30486,24 +30559,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H51" s="100">
+      <c r="H51" s="98">
         <v>0.08</v>
       </c>
-      <c r="I51" s="101" t="e">
+      <c r="I51" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J51" s="102">
+      <c r="J51" s="100">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K51" s="101" t="e">
+      <c r="K51" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L51" s="102">
+      <c r="L51" s="100">
         <v>0.92</v>
       </c>
-      <c r="M51" s="103" t="e">
+      <c r="M51" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30513,24 +30586,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H52" s="100">
+      <c r="H52" s="98">
         <v>0.09</v>
       </c>
-      <c r="I52" s="101" t="e">
+      <c r="I52" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J52" s="102">
+      <c r="J52" s="100">
         <v>0.6</v>
       </c>
-      <c r="K52" s="101" t="e">
+      <c r="K52" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L52" s="102">
+      <c r="L52" s="100">
         <v>0.93</v>
       </c>
-      <c r="M52" s="103" t="e">
+      <c r="M52" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30540,24 +30613,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H53" s="100">
+      <c r="H53" s="98">
         <v>0.1</v>
       </c>
-      <c r="I53" s="101" t="e">
+      <c r="I53" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J53" s="102">
+      <c r="J53" s="100">
         <v>0.65</v>
       </c>
-      <c r="K53" s="101" t="e">
+      <c r="K53" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L53" s="102">
+      <c r="L53" s="100">
         <v>0.94</v>
       </c>
-      <c r="M53" s="103" t="e">
+      <c r="M53" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30567,24 +30640,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H54" s="100">
+      <c r="H54" s="98">
         <v>0.11</v>
       </c>
-      <c r="I54" s="101" t="e">
+      <c r="I54" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J54" s="102">
+      <c r="J54" s="100">
         <v>0.7</v>
       </c>
-      <c r="K54" s="101" t="e">
+      <c r="K54" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L54" s="102">
+      <c r="L54" s="100">
         <v>0.95</v>
       </c>
-      <c r="M54" s="103" t="e">
+      <c r="M54" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30594,24 +30667,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H55" s="100">
+      <c r="H55" s="98">
         <v>0.12</v>
       </c>
-      <c r="I55" s="101" t="e">
+      <c r="I55" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J55" s="102">
+      <c r="J55" s="100">
         <v>0.75</v>
       </c>
-      <c r="K55" s="101" t="e">
+      <c r="K55" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L55" s="102">
+      <c r="L55" s="100">
         <v>0.96</v>
       </c>
-      <c r="M55" s="103" t="e">
+      <c r="M55" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30621,24 +30694,24 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H56" s="100">
+      <c r="H56" s="98">
         <v>0.13</v>
       </c>
-      <c r="I56" s="101" t="e">
+      <c r="I56" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J56" s="102">
+      <c r="J56" s="100">
         <v>0.8</v>
       </c>
-      <c r="K56" s="101" t="e">
+      <c r="K56" s="99" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L56" s="102">
+      <c r="L56" s="100">
         <v>0.97</v>
       </c>
-      <c r="M56" s="103" t="e">
+      <c r="M56" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30648,19 +30721,19 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H57" s="100">
+      <c r="H57" s="98">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I57" s="101" t="e">
+      <c r="I57" s="99" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J57" s="102"/>
-      <c r="K57" s="101"/>
-      <c r="L57" s="102">
+      <c r="J57" s="100"/>
+      <c r="K57" s="99"/>
+      <c r="L57" s="100">
         <v>0.98</v>
       </c>
-      <c r="M57" s="103" t="e">
+      <c r="M57" s="101" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30670,19 +30743,19 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H58" s="104">
+      <c r="H58" s="102">
         <v>0.15</v>
       </c>
-      <c r="I58" s="105" t="e">
+      <c r="I58" s="103" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J58" s="106"/>
-      <c r="K58" s="85"/>
-      <c r="L58" s="107">
+      <c r="J58" s="104"/>
+      <c r="K58" s="83"/>
+      <c r="L58" s="105">
         <v>0.99</v>
       </c>
-      <c r="M58" s="108" t="e">
+      <c r="M58" s="106" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -30698,47 +30771,47 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H60" s="109" t="s">
+      <c r="H60" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="I60" s="110"/>
+      <c r="I60" s="108"/>
     </row>
     <row r="61" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H61" s="111" t="s">
+      <c r="H61" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="I61" s="112"/>
+      <c r="I61" s="110"/>
     </row>
     <row r="62" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H62" s="113"/>
+      <c r="H62" s="111"/>
     </row>
     <row r="63" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H63" s="109" t="s">
+      <c r="H63" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="I63" s="114"/>
+      <c r="I63" s="112"/>
     </row>
     <row r="64" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D64" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H64" s="115" t="s">
+      <c r="H64" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="I64" s="116">
+      <c r="I64" s="114">
         <f>I63*(1-I60)</f>
         <v>0</v>
       </c>
@@ -30748,10 +30821,10 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H65" s="111" t="s">
+      <c r="H65" s="109" t="s">
         <v>121</v>
       </c>
-      <c r="I65" s="117">
+      <c r="I65" s="115">
         <f>I63*(1+I61)</f>
         <v>0</v>
       </c>

</xml_diff>